<commit_message>
Added Definicoes. Idade Minima. Dp_Popup starts v/ ano. Inserir sem data. Alt Design PagPri. Falta Corrigir Cod Post nulo
</commit_message>
<xml_diff>
--- a/PAP.xlsx
+++ b/PAP.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PAP\Trabalhos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A0EE3B2-5DDB-4948-AFB0-BAB84F6CB012}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F9561DB-09DC-4FE0-9F71-4EA4F7C77121}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{8D30B0BE-303C-4698-B2AD-FBEAA77B297E}"/>
   </bookViews>
@@ -220,28 +220,28 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -561,105 +561,105 @@
   <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6:J6"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="F5" s="14" t="s">
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="F5" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="14"/>
+      <c r="G5" s="9"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="F6" s="11" t="s">
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="F6" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
       <c r="K6" s="7" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="F7" s="11" t="s">
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="F7" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
       <c r="K7" s="7" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="F8" s="15" t="s">
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="F8" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
       <c r="K8" s="7" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="F9" s="11" t="s">
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="F9" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
       <c r="K9" s="7" t="s">
         <v>26</v>
       </c>
@@ -668,18 +668,18 @@
       <c r="A10" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="F10" s="12" t="s">
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="F10" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
       <c r="K10" s="7" t="s">
         <v>26</v>
       </c>
@@ -688,18 +688,18 @@
       <c r="A11" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="F11" s="9" t="s">
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="F11" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
       <c r="K11" s="7" t="s">
         <v>26</v>
       </c>
@@ -708,18 +708,18 @@
       <c r="A12" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="F12" s="11" t="s">
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="F12" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
       <c r="K12" s="7" t="s">
         <v>28</v>
       </c>
@@ -728,13 +728,13 @@
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
-      <c r="F13" s="11" t="s">
+      <c r="F13" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
       <c r="K13" s="7" t="s">
         <v>26</v>
       </c>
@@ -743,209 +743,232 @@
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
-      <c r="F14" s="15" t="s">
+      <c r="F14" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="15"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
       <c r="K14" s="7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F15" s="10" t="s">
+      <c r="F15" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="11"/>
       <c r="K15" s="7" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F16" s="10" t="s">
+      <c r="F16" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="10"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
       <c r="K16" s="7" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="17" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="F17" s="15" t="s">
+      <c r="F17" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="G17" s="15"/>
-      <c r="H17" s="15"/>
-      <c r="I17" s="15"/>
-      <c r="J17" s="15"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
       <c r="K17" s="7" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="18" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="F18" s="9" t="s">
+      <c r="F18" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="13"/>
       <c r="K18" s="7" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="19" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="F19" s="11" t="s">
+      <c r="F19" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="11"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
       <c r="K19" s="7" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="20" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="F20" s="9" t="s">
+      <c r="F20" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="13"/>
       <c r="K20" s="7" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="F21" s="12" t="s">
+      <c r="F21" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="12"/>
-      <c r="J21" s="12"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
+      <c r="I21" s="15"/>
+      <c r="J21" s="15"/>
       <c r="K21" s="7" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="22" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="F22" s="10" t="s">
+      <c r="F22" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="G22" s="10"/>
-      <c r="H22" s="10"/>
-      <c r="I22" s="10"/>
-      <c r="J22" s="10"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="11"/>
       <c r="K22" s="7" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="23" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="F23" s="10" t="s">
+      <c r="F23" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="G23" s="10"/>
-      <c r="H23" s="10"/>
-      <c r="I23" s="10"/>
-      <c r="J23" s="10"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="11"/>
       <c r="K23" s="7" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="24" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="F24" s="10" t="s">
+      <c r="F24" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="G24" s="10"/>
-      <c r="H24" s="10"/>
-      <c r="I24" s="10"/>
-      <c r="J24" s="10"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="11"/>
       <c r="K24" s="7" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="25" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="8"/>
-      <c r="J25" s="8"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="10"/>
     </row>
     <row r="26" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
-      <c r="I26" s="8"/>
-      <c r="J26" s="8"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="10"/>
+      <c r="J26" s="10"/>
     </row>
     <row r="27" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="F27" s="8"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="8"/>
-      <c r="I27" s="8"/>
-      <c r="J27" s="8"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="10"/>
     </row>
     <row r="28" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
-      <c r="I28" s="8"/>
-      <c r="J28" s="8"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="10"/>
+      <c r="J28" s="10"/>
     </row>
     <row r="29" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="8"/>
-      <c r="J29" s="8"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="10"/>
+      <c r="I29" s="10"/>
+      <c r="J29" s="10"/>
     </row>
     <row r="30" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="F30" s="8"/>
-      <c r="G30" s="8"/>
-      <c r="H30" s="8"/>
-      <c r="I30" s="8"/>
-      <c r="J30" s="8"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="10"/>
+      <c r="J30" s="10"/>
     </row>
     <row r="31" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="F31" s="8"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="8"/>
-      <c r="I31" s="8"/>
-      <c r="J31" s="8"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="10"/>
+      <c r="J31" s="10"/>
     </row>
     <row r="32" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="F32" s="8"/>
-      <c r="G32" s="8"/>
-      <c r="H32" s="8"/>
-      <c r="I32" s="8"/>
-      <c r="J32" s="8"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="10"/>
+      <c r="I32" s="10"/>
+      <c r="J32" s="10"/>
     </row>
     <row r="33" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F33" s="8"/>
-      <c r="G33" s="8"/>
-      <c r="H33" s="8"/>
-      <c r="I33" s="8"/>
-      <c r="J33" s="8"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="10"/>
+      <c r="I33" s="10"/>
+      <c r="J33" s="10"/>
     </row>
     <row r="34" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F34" s="8"/>
-      <c r="G34" s="8"/>
-      <c r="H34" s="8"/>
-      <c r="I34" s="8"/>
-      <c r="J34" s="8"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="10"/>
+      <c r="H34" s="10"/>
+      <c r="I34" s="10"/>
+      <c r="J34" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="39">
+    <mergeCell ref="F33:J33"/>
+    <mergeCell ref="F20:J20"/>
+    <mergeCell ref="F24:J24"/>
+    <mergeCell ref="F25:J25"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="F22:J22"/>
+    <mergeCell ref="F23:J23"/>
+    <mergeCell ref="F34:J34"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="F28:J28"/>
+    <mergeCell ref="F29:J29"/>
+    <mergeCell ref="F30:J30"/>
+    <mergeCell ref="F31:J31"/>
+    <mergeCell ref="F32:J32"/>
+    <mergeCell ref="F9:J9"/>
+    <mergeCell ref="F10:J10"/>
+    <mergeCell ref="F21:J21"/>
     <mergeCell ref="A1:D2"/>
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="F27:J27"/>
@@ -962,29 +985,6 @@
     <mergeCell ref="F6:J6"/>
     <mergeCell ref="F7:J7"/>
     <mergeCell ref="F8:J8"/>
-    <mergeCell ref="F34:J34"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="F28:J28"/>
-    <mergeCell ref="F29:J29"/>
-    <mergeCell ref="F30:J30"/>
-    <mergeCell ref="F31:J31"/>
-    <mergeCell ref="F32:J32"/>
-    <mergeCell ref="F9:J9"/>
-    <mergeCell ref="F10:J10"/>
-    <mergeCell ref="F21:J21"/>
-    <mergeCell ref="F33:J33"/>
-    <mergeCell ref="F20:J20"/>
-    <mergeCell ref="F24:J24"/>
-    <mergeCell ref="F25:J25"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="F22:J22"/>
-    <mergeCell ref="F23:J23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
alt database, gerirclientes, gerirtrabalhos, gerirservicos and others.
</commit_message>
<xml_diff>
--- a/PAP.xlsx
+++ b/PAP.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PAP\Trabalhos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F9561DB-09DC-4FE0-9F71-4EA4F7C77121}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05F26A2F-3562-417B-9A6C-1CB5E915206C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{8D30B0BE-303C-4698-B2AD-FBEAA77B297E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{8D30B0BE-303C-4698-B2AD-FBEAA77B297E}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="34">
   <si>
     <t>Tester PAP</t>
   </si>
@@ -121,6 +121,12 @@
   </si>
   <si>
     <t>Concluido</t>
+  </si>
+  <si>
+    <t>NR</t>
+  </si>
+  <si>
+    <t>Não Resolver</t>
   </si>
 </sst>
 </file>
@@ -220,28 +226,28 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -561,145 +567,145 @@
   <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="F5" s="9" t="s">
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="F5" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="9"/>
+      <c r="G5" s="14"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="F6" s="14" t="s">
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="F6" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
       <c r="K6" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="F7" s="14" t="s">
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="F7" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
       <c r="K7" s="7" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="F8" s="12" t="s">
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="F8" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
       <c r="K8" s="7" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="F9" s="14" t="s">
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="F9" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
       <c r="K9" s="7" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="F10" s="15" t="s">
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="F10" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="15"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
       <c r="K10" s="7" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="F11" s="13" t="s">
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="F11" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
       <c r="K11" s="7" t="s">
         <v>26</v>
       </c>
@@ -708,251 +714,265 @@
       <c r="A12" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="F12" s="14" t="s">
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="F12" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
       <c r="K12" s="7" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="F13" s="14" t="s">
+      <c r="A13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="F13" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
       <c r="K13" s="7" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
-      <c r="F14" s="12" t="s">
+      <c r="F14" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15"/>
       <c r="K14" s="7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F15" s="11" t="s">
+      <c r="F15" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="11"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
       <c r="K15" s="7" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F16" s="11" t="s">
+      <c r="F16" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
       <c r="K16" s="7" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="17" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="F17" s="12" t="s">
+      <c r="F17" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="12"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
       <c r="K17" s="7" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="F18" s="13" t="s">
+      <c r="F18" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
       <c r="K18" s="7" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="F19" s="14" t="s">
+      <c r="F19" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
       <c r="K19" s="7" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="20" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="F20" s="13" t="s">
+      <c r="F20" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
       <c r="K20" s="7" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="21" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="F21" s="15" t="s">
+      <c r="F21" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="G21" s="15"/>
-      <c r="H21" s="15"/>
-      <c r="I21" s="15"/>
-      <c r="J21" s="15"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
       <c r="K21" s="7" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="22" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="F22" s="11" t="s">
+      <c r="F22" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="11"/>
-      <c r="J22" s="11"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
       <c r="K22" s="7" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="23" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="F23" s="11" t="s">
+      <c r="F23" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="11"/>
-      <c r="J23" s="11"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="10"/>
       <c r="K23" s="7" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="24" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="F24" s="11" t="s">
+      <c r="F24" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="11"/>
-      <c r="J24" s="11"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="10"/>
       <c r="K24" s="7" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="25" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="F25" s="10"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="10"/>
-      <c r="I25" s="10"/>
-      <c r="J25" s="10"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8"/>
     </row>
     <row r="26" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="F26" s="10"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="10"/>
-      <c r="I26" s="10"/>
-      <c r="J26" s="10"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="8"/>
     </row>
     <row r="27" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="10"/>
-      <c r="I27" s="10"/>
-      <c r="J27" s="10"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="8"/>
     </row>
     <row r="28" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="F28" s="10"/>
-      <c r="G28" s="10"/>
-      <c r="H28" s="10"/>
-      <c r="I28" s="10"/>
-      <c r="J28" s="10"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
+      <c r="I28" s="8"/>
+      <c r="J28" s="8"/>
     </row>
     <row r="29" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="F29" s="10"/>
-      <c r="G29" s="10"/>
-      <c r="H29" s="10"/>
-      <c r="I29" s="10"/>
-      <c r="J29" s="10"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="8"/>
     </row>
     <row r="30" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="F30" s="10"/>
-      <c r="G30" s="10"/>
-      <c r="H30" s="10"/>
-      <c r="I30" s="10"/>
-      <c r="J30" s="10"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="8"/>
+      <c r="J30" s="8"/>
     </row>
     <row r="31" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="F31" s="10"/>
-      <c r="G31" s="10"/>
-      <c r="H31" s="10"/>
-      <c r="I31" s="10"/>
-      <c r="J31" s="10"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="8"/>
+      <c r="J31" s="8"/>
     </row>
     <row r="32" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="F32" s="10"/>
-      <c r="G32" s="10"/>
-      <c r="H32" s="10"/>
-      <c r="I32" s="10"/>
-      <c r="J32" s="10"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="8"/>
+      <c r="H32" s="8"/>
+      <c r="I32" s="8"/>
+      <c r="J32" s="8"/>
     </row>
     <row r="33" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F33" s="10"/>
-      <c r="G33" s="10"/>
-      <c r="H33" s="10"/>
-      <c r="I33" s="10"/>
-      <c r="J33" s="10"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="8"/>
+      <c r="I33" s="8"/>
+      <c r="J33" s="8"/>
     </row>
     <row r="34" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F34" s="10"/>
-      <c r="G34" s="10"/>
-      <c r="H34" s="10"/>
-      <c r="I34" s="10"/>
-      <c r="J34" s="10"/>
+      <c r="F34" s="8"/>
+      <c r="G34" s="8"/>
+      <c r="H34" s="8"/>
+      <c r="I34" s="8"/>
+      <c r="J34" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="39">
-    <mergeCell ref="F33:J33"/>
-    <mergeCell ref="F20:J20"/>
-    <mergeCell ref="F24:J24"/>
-    <mergeCell ref="F25:J25"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="F22:J22"/>
-    <mergeCell ref="F23:J23"/>
+  <mergeCells count="40">
+    <mergeCell ref="A1:D2"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F27:J27"/>
+    <mergeCell ref="F16:J16"/>
+    <mergeCell ref="F17:J17"/>
+    <mergeCell ref="F18:J18"/>
+    <mergeCell ref="F19:J19"/>
+    <mergeCell ref="F11:J11"/>
+    <mergeCell ref="F12:J12"/>
+    <mergeCell ref="F13:J13"/>
+    <mergeCell ref="F14:J14"/>
+    <mergeCell ref="F26:J26"/>
+    <mergeCell ref="F15:J15"/>
+    <mergeCell ref="F6:J6"/>
+    <mergeCell ref="F7:J7"/>
+    <mergeCell ref="F8:J8"/>
     <mergeCell ref="F34:J34"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="B7:D7"/>
@@ -969,22 +989,14 @@
     <mergeCell ref="F9:J9"/>
     <mergeCell ref="F10:J10"/>
     <mergeCell ref="F21:J21"/>
-    <mergeCell ref="A1:D2"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="F27:J27"/>
-    <mergeCell ref="F16:J16"/>
-    <mergeCell ref="F17:J17"/>
-    <mergeCell ref="F18:J18"/>
-    <mergeCell ref="F19:J19"/>
-    <mergeCell ref="F11:J11"/>
-    <mergeCell ref="F12:J12"/>
-    <mergeCell ref="F13:J13"/>
-    <mergeCell ref="F14:J14"/>
-    <mergeCell ref="F26:J26"/>
-    <mergeCell ref="F15:J15"/>
-    <mergeCell ref="F6:J6"/>
-    <mergeCell ref="F7:J7"/>
-    <mergeCell ref="F8:J8"/>
+    <mergeCell ref="F33:J33"/>
+    <mergeCell ref="F20:J20"/>
+    <mergeCell ref="F24:J24"/>
+    <mergeCell ref="F25:J25"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="F22:J22"/>
+    <mergeCell ref="F23:J23"/>
+    <mergeCell ref="B13:D13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>